<commit_message>
re organizar tabla de contenido
</commit_message>
<xml_diff>
--- a/temario.xlsx
+++ b/temario.xlsx
@@ -1,18 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\home\jacobo\Documentos\estadias\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tesina\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{472B5A2A-5327-4E77-BACE-579B441DC1A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1125" windowWidth="20490" windowHeight="7890"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="135">
   <si>
     <t>Introducción conceptos basicos</t>
   </si>
@@ -297,13 +299,145 @@
   </si>
   <si>
     <t>Oracle Cloud Platform Application Integration 2021 Specialist 1Z0-1042-21</t>
+  </si>
+  <si>
+    <t>Actividades</t>
+  </si>
+  <si>
+    <t>Meses</t>
+  </si>
+  <si>
+    <t>Enero</t>
+  </si>
+  <si>
+    <t>Febrero</t>
+  </si>
+  <si>
+    <t>Marzo</t>
+  </si>
+  <si>
+    <t>Abril</t>
+  </si>
+  <si>
+    <t>1. Crear un modelo de 10 tablas</t>
+  </si>
+  <si>
+    <t>3. Reporte Ordenes de compra</t>
+  </si>
+  <si>
+    <t>4. Conexiones SOAP,REST,SFTP,ERP</t>
+  </si>
+  <si>
+    <t>OIC</t>
+  </si>
+  <si>
+    <t>2. Consultas avanzadas</t>
+  </si>
+  <si>
+    <t>8. Configuracion de servicio de conexión.</t>
+  </si>
+  <si>
+    <t>Visual Builder</t>
+  </si>
+  <si>
+    <t>7.Crear facturas mediante FBDI con adapter ERP cloud.</t>
+  </si>
+  <si>
+    <t>5.Extraccion de datos archivos mediante conexión a SFTP.</t>
+  </si>
+  <si>
+    <t>6.Consumo de reportes de OTBI con servicio SOAP</t>
+  </si>
+  <si>
+    <t>9. Ejecucion de proceso desde pantalla</t>
+  </si>
+  <si>
+    <t>10. Pantalla que obtenga informacion de integraciones</t>
+  </si>
+  <si>
+    <t>11. Pantalla que muestre datos con un business object</t>
+  </si>
+  <si>
+    <t>SOACS</t>
+  </si>
+  <si>
+    <t>12. Composite que muestre un valor predeermiando</t>
+  </si>
+  <si>
+    <t>13. Configuracion de dataSource de BD</t>
+  </si>
+  <si>
+    <t>14. Configuracion de Ftp adapter</t>
+  </si>
+  <si>
+    <t>15. Composite para hacer uso de objetos de BD</t>
+  </si>
+  <si>
+    <t>16. Composite que crea archivos en servidor mediante una cadena Base64</t>
+  </si>
+  <si>
+    <t>Process Aplication</t>
+  </si>
+  <si>
+    <t>17. proceso estructurado y creando un modelo de decisión</t>
+  </si>
+  <si>
+    <t>18. Creacion de una app utilizando QuickStart</t>
+  </si>
+  <si>
+    <t>19. Proceso dinamico utilizando reglas de negocio</t>
+  </si>
+  <si>
+    <t>20. Creacion de una app iniciando desde un fromulario</t>
+  </si>
+  <si>
+    <t>21. Consultas avanzadas</t>
+  </si>
+  <si>
+    <t>Oracle SQL/PLSQP</t>
+  </si>
+  <si>
+    <t>22. Creación de funciones</t>
+  </si>
+  <si>
+    <t>23. Creación de procedimientos</t>
+  </si>
+  <si>
+    <t>24. Paquetes</t>
+  </si>
+  <si>
+    <t>25. Data model Ordenes de compra</t>
+  </si>
+  <si>
+    <t>BI PUBLISHER</t>
+  </si>
+  <si>
+    <t>26. Reporte Ordenes de compra</t>
+  </si>
+  <si>
+    <t>27. Creación de Dashboard</t>
+  </si>
+  <si>
+    <t>28. Rroceso programado</t>
+  </si>
+  <si>
+    <t>29. Reporte con BI Publisher</t>
+  </si>
+  <si>
+    <t>ODI</t>
+  </si>
+  <si>
+    <t>30. Creacion de modelos y topologias</t>
+  </si>
+  <si>
+    <t>31. Planificación de escenarios</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -311,16 +445,71 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808080"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA6A6A6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -328,13 +517,158 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -614,482 +948,482 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C3:G95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E98" sqref="E98"/>
+    <sheetView topLeftCell="B61" workbookViewId="0">
+      <selection activeCell="G92" sqref="G92"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="23.75" customWidth="1"/>
-    <col min="6" max="6" width="8.25" customWidth="1"/>
+    <col min="5" max="5" width="23.7109375" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:6">
+    <row r="3" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="3:6">
+    <row r="4" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="3:6">
+    <row r="5" spans="3:6" x14ac:dyDescent="0.25">
       <c r="E5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="3:6">
+    <row r="6" spans="3:6" x14ac:dyDescent="0.25">
       <c r="E6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="3:6">
+    <row r="7" spans="3:6" x14ac:dyDescent="0.25">
       <c r="F7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="3:6">
+    <row r="8" spans="3:6" x14ac:dyDescent="0.25">
       <c r="F8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="3:6">
+    <row r="9" spans="3:6" x14ac:dyDescent="0.25">
       <c r="E9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="3:6">
+    <row r="10" spans="3:6" x14ac:dyDescent="0.25">
       <c r="F10" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="3:6">
+    <row r="11" spans="3:6" x14ac:dyDescent="0.25">
       <c r="F11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="3:6">
+    <row r="12" spans="3:6" x14ac:dyDescent="0.25">
       <c r="F12" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="3:6">
+    <row r="13" spans="3:6" x14ac:dyDescent="0.25">
       <c r="F13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="3:6">
+    <row r="14" spans="3:6" x14ac:dyDescent="0.25">
       <c r="E14" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="3:6">
+    <row r="15" spans="3:6" x14ac:dyDescent="0.25">
       <c r="E15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="3:6">
+    <row r="16" spans="3:6" x14ac:dyDescent="0.25">
       <c r="E16" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="4:5">
+    <row r="17" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="4:5">
+    <row r="18" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E18" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="4:5">
+    <row r="19" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E19" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="4:5">
+    <row r="20" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E20" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="4:5">
+    <row r="21" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E21" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="4:5">
+    <row r="22" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E22" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="4:5">
+    <row r="23" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E23" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="4:5">
+    <row r="24" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E24" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="4:5">
+    <row r="25" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E25" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="4:5">
+    <row r="26" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D26" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="4:5">
+    <row r="27" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E27" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="4:5">
+    <row r="28" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E28" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="4:5">
+    <row r="29" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D29" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="4:5">
+    <row r="30" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E30" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="4:5">
+    <row r="31" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E31" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="4:5">
+    <row r="32" spans="4:5" x14ac:dyDescent="0.25">
       <c r="E32" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="3:6">
+    <row r="33" spans="3:6" x14ac:dyDescent="0.25">
       <c r="E33" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="3:6">
+    <row r="34" spans="3:6" x14ac:dyDescent="0.25">
       <c r="E34" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="35" spans="3:6">
+    <row r="35" spans="3:6" x14ac:dyDescent="0.25">
       <c r="E35" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="3:6">
+    <row r="36" spans="3:6" x14ac:dyDescent="0.25">
       <c r="E36" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="3:6">
+    <row r="37" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D37" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="3:6">
+    <row r="38" spans="3:6" x14ac:dyDescent="0.25">
       <c r="E38" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="3:6">
+    <row r="39" spans="3:6" x14ac:dyDescent="0.25">
       <c r="E39" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="3:6">
+    <row r="40" spans="3:6" x14ac:dyDescent="0.25">
       <c r="E40" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="3:6">
+    <row r="41" spans="3:6" x14ac:dyDescent="0.25">
       <c r="E41" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="42" spans="3:6">
+    <row r="42" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C42" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="43" spans="3:6">
+    <row r="43" spans="3:6" x14ac:dyDescent="0.25">
       <c r="D43" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="3:6">
+    <row r="44" spans="3:6" x14ac:dyDescent="0.25">
       <c r="E44" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="45" spans="3:6">
+    <row r="45" spans="3:6" x14ac:dyDescent="0.25">
       <c r="F45" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="46" spans="3:6">
+    <row r="46" spans="3:6" x14ac:dyDescent="0.25">
       <c r="F46" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="47" spans="3:6">
+    <row r="47" spans="3:6" x14ac:dyDescent="0.25">
       <c r="F47" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="48" spans="3:6">
+    <row r="48" spans="3:6" x14ac:dyDescent="0.25">
       <c r="F48" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="49" spans="5:7">
+    <row r="49" spans="5:7" x14ac:dyDescent="0.25">
       <c r="F49" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="50" spans="5:7">
+    <row r="50" spans="5:7" x14ac:dyDescent="0.25">
       <c r="G50" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="51" spans="5:7">
+    <row r="51" spans="5:7" x14ac:dyDescent="0.25">
       <c r="G51" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="52" spans="5:7">
+    <row r="52" spans="5:7" x14ac:dyDescent="0.25">
       <c r="G52" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="53" spans="5:7">
+    <row r="53" spans="5:7" x14ac:dyDescent="0.25">
       <c r="G53" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="54" spans="5:7">
+    <row r="54" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E54" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="55" spans="5:7">
+    <row r="55" spans="5:7" x14ac:dyDescent="0.25">
       <c r="F55" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="56" spans="5:7">
+    <row r="56" spans="5:7" x14ac:dyDescent="0.25">
       <c r="F56" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="57" spans="5:7">
+    <row r="57" spans="5:7" x14ac:dyDescent="0.25">
       <c r="F57" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="58" spans="5:7">
+    <row r="58" spans="5:7" x14ac:dyDescent="0.25">
       <c r="F58" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="59" spans="5:7">
+    <row r="59" spans="5:7" x14ac:dyDescent="0.25">
       <c r="G59" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="60" spans="5:7">
+    <row r="60" spans="5:7" x14ac:dyDescent="0.25">
       <c r="G60" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="61" spans="5:7">
+    <row r="61" spans="5:7" x14ac:dyDescent="0.25">
       <c r="G61" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="62" spans="5:7">
+    <row r="62" spans="5:7" x14ac:dyDescent="0.25">
       <c r="G62" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="63" spans="5:7">
+    <row r="63" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E63" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="64" spans="5:7">
+    <row r="64" spans="5:7" x14ac:dyDescent="0.25">
       <c r="F64" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="65" spans="5:7">
+    <row r="65" spans="5:7" x14ac:dyDescent="0.25">
       <c r="F65" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="66" spans="5:7">
+    <row r="66" spans="5:7" x14ac:dyDescent="0.25">
       <c r="F66" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="67" spans="5:7">
+    <row r="67" spans="5:7" x14ac:dyDescent="0.25">
       <c r="F67" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="68" spans="5:7">
+    <row r="68" spans="5:7" x14ac:dyDescent="0.25">
       <c r="F68" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="69" spans="5:7">
+    <row r="69" spans="5:7" x14ac:dyDescent="0.25">
       <c r="G69" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="70" spans="5:7">
+    <row r="70" spans="5:7" x14ac:dyDescent="0.25">
       <c r="G70" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="71" spans="5:7">
+    <row r="71" spans="5:7" x14ac:dyDescent="0.25">
       <c r="G71" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="72" spans="5:7">
+    <row r="72" spans="5:7" x14ac:dyDescent="0.25">
       <c r="G72" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="73" spans="5:7">
+    <row r="73" spans="5:7" x14ac:dyDescent="0.25">
       <c r="G73" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="74" spans="5:7">
+    <row r="74" spans="5:7" x14ac:dyDescent="0.25">
       <c r="G74" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="75" spans="5:7">
+    <row r="75" spans="5:7" x14ac:dyDescent="0.25">
       <c r="E75" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="76" spans="5:7">
+    <row r="76" spans="5:7" x14ac:dyDescent="0.25">
       <c r="F76" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="77" spans="5:7">
+    <row r="77" spans="5:7" x14ac:dyDescent="0.25">
       <c r="F77" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="78" spans="5:7">
+    <row r="78" spans="5:7" x14ac:dyDescent="0.25">
       <c r="F78" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="79" spans="5:7">
+    <row r="79" spans="5:7" x14ac:dyDescent="0.25">
       <c r="F79" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="80" spans="5:7">
+    <row r="80" spans="5:7" x14ac:dyDescent="0.25">
       <c r="F80" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="81" spans="3:7">
+    <row r="81" spans="3:7" x14ac:dyDescent="0.25">
       <c r="E81" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="82" spans="3:7">
+    <row r="82" spans="3:7" x14ac:dyDescent="0.25">
       <c r="F82" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="83" spans="3:7">
+    <row r="83" spans="3:7" x14ac:dyDescent="0.25">
       <c r="F83" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="84" spans="3:7">
+    <row r="84" spans="3:7" x14ac:dyDescent="0.25">
       <c r="F84" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="85" spans="3:7">
+    <row r="85" spans="3:7" x14ac:dyDescent="0.25">
       <c r="F85" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="86" spans="3:7">
+    <row r="86" spans="3:7" x14ac:dyDescent="0.25">
       <c r="F86" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="87" spans="3:7">
+    <row r="87" spans="3:7" x14ac:dyDescent="0.25">
       <c r="F87" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="88" spans="3:7">
+    <row r="88" spans="3:7" x14ac:dyDescent="0.25">
       <c r="F88" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="89" spans="3:7">
+    <row r="89" spans="3:7" x14ac:dyDescent="0.25">
       <c r="G89" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="90" spans="3:7">
+    <row r="90" spans="3:7" x14ac:dyDescent="0.25">
       <c r="G90" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="91" spans="3:7">
+    <row r="91" spans="3:7" x14ac:dyDescent="0.25">
       <c r="G91" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="92" spans="3:7">
+    <row r="92" spans="3:7" x14ac:dyDescent="0.25">
       <c r="G92" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="93" spans="3:7">
+    <row r="93" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C93" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="94" spans="3:7">
+    <row r="94" spans="3:7" x14ac:dyDescent="0.25">
       <c r="E94" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="95" spans="3:7">
+    <row r="95" spans="3:7" x14ac:dyDescent="0.25">
       <c r="E95" t="s">
         <v>90</v>
       </c>
@@ -1097,4 +1431,995 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56849E69-8D35-4112-94FE-72BBBD3BEE48}">
+  <dimension ref="D3:T47"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="39.140625" customWidth="1"/>
+    <col min="5" max="20" width="3.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="4:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="4:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D4" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8"/>
+      <c r="O4" s="8"/>
+      <c r="P4" s="8"/>
+      <c r="Q4" s="8"/>
+      <c r="R4" s="8"/>
+      <c r="S4" s="8"/>
+      <c r="T4" s="10"/>
+    </row>
+    <row r="5" spans="4:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D5" s="6"/>
+      <c r="E5" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="N5" s="12"/>
+      <c r="O5" s="12"/>
+      <c r="P5" s="13"/>
+      <c r="Q5" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="R5" s="12"/>
+      <c r="S5" s="12"/>
+      <c r="T5" s="13"/>
+    </row>
+    <row r="6" spans="4:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D6" s="7"/>
+      <c r="E6" s="2">
+        <v>1</v>
+      </c>
+      <c r="F6" s="2">
+        <v>2</v>
+      </c>
+      <c r="G6" s="2">
+        <v>3</v>
+      </c>
+      <c r="H6" s="2">
+        <v>4</v>
+      </c>
+      <c r="I6" s="2">
+        <v>1</v>
+      </c>
+      <c r="J6" s="2">
+        <v>2</v>
+      </c>
+      <c r="K6" s="2">
+        <v>3</v>
+      </c>
+      <c r="L6" s="2">
+        <v>4</v>
+      </c>
+      <c r="M6" s="2">
+        <v>1</v>
+      </c>
+      <c r="N6" s="2">
+        <v>2</v>
+      </c>
+      <c r="O6" s="2">
+        <v>3</v>
+      </c>
+      <c r="P6" s="2">
+        <v>4</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>1</v>
+      </c>
+      <c r="R6" s="2">
+        <v>2</v>
+      </c>
+      <c r="S6" s="2">
+        <v>3</v>
+      </c>
+      <c r="T6" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="4:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D7" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="19"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="19"/>
+      <c r="L7" s="19"/>
+      <c r="M7" s="19"/>
+      <c r="N7" s="19"/>
+      <c r="O7" s="19"/>
+      <c r="P7" s="19"/>
+      <c r="Q7" s="19"/>
+      <c r="R7" s="19"/>
+      <c r="S7" s="19"/>
+      <c r="T7" s="19"/>
+    </row>
+    <row r="8" spans="4:20" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D8" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="E8" s="14"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="4"/>
+      <c r="R8" s="4"/>
+      <c r="S8" s="4"/>
+      <c r="T8" s="4"/>
+    </row>
+    <row r="9" spans="4:20" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D9" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E9" s="14"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
+      <c r="M9" s="4"/>
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
+      <c r="Q9" s="4"/>
+      <c r="R9" s="4"/>
+      <c r="S9" s="4"/>
+      <c r="T9" s="4"/>
+    </row>
+    <row r="10" spans="4:20" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D10" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E10" s="14"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
+      <c r="M10" s="4"/>
+      <c r="N10" s="4"/>
+      <c r="O10" s="4"/>
+      <c r="P10" s="4"/>
+      <c r="Q10" s="4"/>
+      <c r="R10" s="4"/>
+      <c r="S10" s="4"/>
+      <c r="T10" s="4"/>
+    </row>
+    <row r="11" spans="4:20" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D11" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="E11" s="15"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
+      <c r="M11" s="4"/>
+      <c r="N11" s="4"/>
+      <c r="O11" s="4"/>
+      <c r="P11" s="4"/>
+      <c r="Q11" s="4"/>
+      <c r="R11" s="4"/>
+      <c r="S11" s="4"/>
+      <c r="T11" s="4"/>
+    </row>
+    <row r="12" spans="4:20" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D12" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E12" s="4"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="4"/>
+      <c r="R12" s="4"/>
+      <c r="S12" s="4"/>
+      <c r="T12" s="4"/>
+    </row>
+    <row r="13" spans="4:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D13" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E13" s="4"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="4"/>
+      <c r="R13" s="4"/>
+      <c r="S13" s="4"/>
+      <c r="T13" s="4"/>
+    </row>
+    <row r="14" spans="4:20" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D14" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="E14" s="4"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="4"/>
+      <c r="O14" s="4"/>
+      <c r="P14" s="4"/>
+      <c r="Q14" s="4"/>
+      <c r="R14" s="4"/>
+      <c r="S14" s="4"/>
+      <c r="T14" s="4"/>
+    </row>
+    <row r="15" spans="4:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D15" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="E15" s="4"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="4"/>
+      <c r="O15" s="4"/>
+      <c r="P15" s="4"/>
+      <c r="Q15" s="4"/>
+      <c r="R15" s="4"/>
+      <c r="S15" s="4"/>
+      <c r="T15" s="4"/>
+    </row>
+    <row r="16" spans="4:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D16" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="E16" s="4"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
+      <c r="O16" s="4"/>
+      <c r="P16" s="4"/>
+      <c r="Q16" s="4"/>
+      <c r="R16" s="4"/>
+      <c r="S16" s="4"/>
+      <c r="T16" s="4"/>
+    </row>
+    <row r="17" spans="4:20" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D17" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="4"/>
+      <c r="M17" s="4"/>
+      <c r="N17" s="4"/>
+      <c r="O17" s="4"/>
+      <c r="P17" s="4"/>
+      <c r="Q17" s="4"/>
+      <c r="R17" s="4"/>
+      <c r="S17" s="4"/>
+      <c r="T17" s="4"/>
+    </row>
+    <row r="18" spans="4:20" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D18" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="4"/>
+      <c r="P18" s="4"/>
+      <c r="Q18" s="4"/>
+      <c r="R18" s="4"/>
+      <c r="S18" s="4"/>
+      <c r="T18" s="4"/>
+    </row>
+    <row r="19" spans="4:20" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D19" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="4"/>
+      <c r="M19" s="4"/>
+      <c r="N19" s="4"/>
+      <c r="O19" s="4"/>
+      <c r="P19" s="4"/>
+      <c r="Q19" s="4"/>
+      <c r="R19" s="4"/>
+      <c r="S19" s="4"/>
+      <c r="T19" s="4"/>
+    </row>
+    <row r="20" spans="4:20" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D20" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="4"/>
+      <c r="O20" s="4"/>
+      <c r="P20" s="4"/>
+      <c r="Q20" s="4"/>
+      <c r="R20" s="4"/>
+      <c r="S20" s="4"/>
+      <c r="T20" s="4"/>
+    </row>
+    <row r="21" spans="4:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D21" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="E21" s="4"/>
+      <c r="F21" s="15"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
+      <c r="N21" s="4"/>
+      <c r="O21" s="4"/>
+      <c r="P21" s="4"/>
+      <c r="Q21" s="4"/>
+      <c r="R21" s="4"/>
+      <c r="S21" s="4"/>
+      <c r="T21" s="4"/>
+    </row>
+    <row r="22" spans="4:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D22" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
+      <c r="N22" s="4"/>
+      <c r="O22" s="4"/>
+      <c r="P22" s="4"/>
+      <c r="Q22" s="4"/>
+      <c r="R22" s="4"/>
+      <c r="S22" s="4"/>
+      <c r="T22" s="4"/>
+    </row>
+    <row r="23" spans="4:20" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D23" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="4"/>
+      <c r="M23" s="4"/>
+      <c r="N23" s="4"/>
+      <c r="O23" s="4"/>
+      <c r="P23" s="4"/>
+      <c r="Q23" s="4"/>
+      <c r="R23" s="4"/>
+      <c r="S23" s="4"/>
+      <c r="T23" s="4"/>
+    </row>
+    <row r="24" spans="4:20" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D24" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="14"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="4"/>
+      <c r="M24" s="4"/>
+      <c r="N24" s="4"/>
+      <c r="O24" s="4"/>
+      <c r="P24" s="4"/>
+      <c r="Q24" s="4"/>
+      <c r="R24" s="4"/>
+      <c r="S24" s="4"/>
+      <c r="T24" s="4"/>
+    </row>
+    <row r="25" spans="4:20" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D25" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="15"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="14"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="4"/>
+      <c r="M25" s="4"/>
+      <c r="N25" s="4"/>
+      <c r="O25" s="4"/>
+      <c r="P25" s="4"/>
+      <c r="Q25" s="4"/>
+      <c r="R25" s="4"/>
+      <c r="S25" s="4"/>
+      <c r="T25" s="4"/>
+    </row>
+    <row r="26" spans="4:20" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D26" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="15"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="14"/>
+      <c r="K26" s="4"/>
+      <c r="L26" s="4"/>
+      <c r="M26" s="4"/>
+      <c r="N26" s="4"/>
+      <c r="O26" s="4"/>
+      <c r="P26" s="4"/>
+      <c r="Q26" s="4"/>
+      <c r="R26" s="4"/>
+      <c r="S26" s="4"/>
+      <c r="T26" s="4"/>
+    </row>
+    <row r="27" spans="4:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D27" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="E27" s="4"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="20"/>
+      <c r="K27" s="4"/>
+      <c r="L27" s="4"/>
+      <c r="M27" s="4"/>
+      <c r="N27" s="4"/>
+      <c r="O27" s="4"/>
+      <c r="P27" s="4"/>
+      <c r="Q27" s="4"/>
+      <c r="R27" s="4"/>
+      <c r="S27" s="4"/>
+      <c r="T27" s="4"/>
+    </row>
+    <row r="28" spans="4:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D28" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="E28" s="4"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="15"/>
+      <c r="K28" s="4"/>
+      <c r="L28" s="4"/>
+      <c r="M28" s="4"/>
+      <c r="N28" s="4"/>
+      <c r="O28" s="4"/>
+      <c r="P28" s="4"/>
+      <c r="Q28" s="4"/>
+      <c r="R28" s="4"/>
+      <c r="S28" s="4"/>
+      <c r="T28" s="4"/>
+    </row>
+    <row r="29" spans="4:20" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D29" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="15"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="4"/>
+      <c r="K29" s="14"/>
+      <c r="L29" s="4"/>
+      <c r="M29" s="4"/>
+      <c r="N29" s="4"/>
+      <c r="O29" s="4"/>
+      <c r="P29" s="4"/>
+      <c r="Q29" s="4"/>
+      <c r="R29" s="4"/>
+      <c r="S29" s="4"/>
+      <c r="T29" s="4"/>
+    </row>
+    <row r="30" spans="4:20" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D30" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="15"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="4"/>
+      <c r="K30" s="14"/>
+      <c r="L30" s="4"/>
+      <c r="M30" s="4"/>
+      <c r="N30" s="4"/>
+      <c r="O30" s="4"/>
+      <c r="P30" s="4"/>
+      <c r="Q30" s="4"/>
+      <c r="R30" s="4"/>
+      <c r="S30" s="4"/>
+      <c r="T30" s="4"/>
+    </row>
+    <row r="31" spans="4:20" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D31" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="15"/>
+      <c r="I31" s="4"/>
+      <c r="J31" s="4"/>
+      <c r="K31" s="4"/>
+      <c r="L31" s="14"/>
+      <c r="M31" s="4"/>
+      <c r="N31" s="4"/>
+      <c r="O31" s="4"/>
+      <c r="P31" s="4"/>
+      <c r="Q31" s="4"/>
+      <c r="R31" s="4"/>
+      <c r="S31" s="4"/>
+      <c r="T31" s="4"/>
+    </row>
+    <row r="32" spans="4:20" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D32" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="15"/>
+      <c r="I32" s="4"/>
+      <c r="J32" s="4"/>
+      <c r="K32" s="4"/>
+      <c r="L32" s="14"/>
+      <c r="M32" s="4"/>
+      <c r="N32" s="4"/>
+      <c r="O32" s="4"/>
+      <c r="P32" s="4"/>
+      <c r="Q32" s="4"/>
+      <c r="R32" s="4"/>
+      <c r="S32" s="4"/>
+      <c r="T32" s="4"/>
+    </row>
+    <row r="33" spans="4:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D33" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="E33" s="4"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4"/>
+      <c r="I33" s="4"/>
+      <c r="J33" s="15"/>
+      <c r="K33" s="4"/>
+      <c r="L33" s="4"/>
+      <c r="M33" s="4"/>
+      <c r="N33" s="4"/>
+      <c r="O33" s="4"/>
+      <c r="P33" s="4"/>
+      <c r="Q33" s="4"/>
+      <c r="R33" s="4"/>
+      <c r="S33" s="4"/>
+      <c r="T33" s="4"/>
+    </row>
+    <row r="34" spans="4:20" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D34" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="15"/>
+      <c r="I34" s="4"/>
+      <c r="J34" s="4"/>
+      <c r="K34" s="4"/>
+      <c r="L34" s="4"/>
+      <c r="M34" s="14"/>
+      <c r="N34" s="15"/>
+      <c r="O34" s="4"/>
+      <c r="P34" s="4"/>
+      <c r="Q34" s="4"/>
+      <c r="R34" s="4"/>
+      <c r="S34" s="4"/>
+      <c r="T34" s="4"/>
+    </row>
+    <row r="35" spans="4:20" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D35" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="15"/>
+      <c r="I35" s="4"/>
+      <c r="J35" s="4"/>
+      <c r="K35" s="4"/>
+      <c r="L35" s="4"/>
+      <c r="M35" s="4"/>
+      <c r="N35" s="14"/>
+      <c r="O35" s="21"/>
+      <c r="P35" s="4"/>
+      <c r="Q35" s="4"/>
+      <c r="R35" s="4"/>
+      <c r="S35" s="4"/>
+      <c r="T35" s="4"/>
+    </row>
+    <row r="36" spans="4:20" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D36" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="15"/>
+      <c r="I36" s="4"/>
+      <c r="J36" s="4"/>
+      <c r="K36" s="4"/>
+      <c r="L36" s="4"/>
+      <c r="M36" s="4"/>
+      <c r="N36" s="14"/>
+      <c r="O36" s="21"/>
+      <c r="P36" s="4"/>
+      <c r="Q36" s="4"/>
+      <c r="R36" s="4"/>
+      <c r="S36" s="4"/>
+      <c r="T36" s="4"/>
+    </row>
+    <row r="37" spans="4:20" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D37" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="15"/>
+      <c r="I37" s="4"/>
+      <c r="J37" s="4"/>
+      <c r="K37" s="4"/>
+      <c r="L37" s="4"/>
+      <c r="M37" s="4"/>
+      <c r="N37" s="14"/>
+      <c r="O37" s="21"/>
+      <c r="P37" s="4"/>
+      <c r="Q37" s="4"/>
+      <c r="R37" s="4"/>
+      <c r="S37" s="4"/>
+      <c r="T37" s="4"/>
+    </row>
+    <row r="38" spans="4:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D38" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="E38" s="4"/>
+      <c r="F38" s="15"/>
+      <c r="G38" s="4"/>
+      <c r="H38" s="4"/>
+      <c r="I38" s="4"/>
+      <c r="J38" s="15"/>
+      <c r="K38" s="4"/>
+      <c r="L38" s="4"/>
+      <c r="M38" s="4"/>
+      <c r="N38" s="4"/>
+      <c r="O38" s="4"/>
+      <c r="P38" s="4"/>
+      <c r="Q38" s="4"/>
+      <c r="R38" s="4"/>
+      <c r="S38" s="4"/>
+      <c r="T38" s="4"/>
+    </row>
+    <row r="39" spans="4:20" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D39" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
+      <c r="H39" s="15"/>
+      <c r="I39" s="4"/>
+      <c r="J39" s="4"/>
+      <c r="K39" s="4"/>
+      <c r="L39" s="4"/>
+      <c r="M39" s="4"/>
+      <c r="N39" s="4"/>
+      <c r="O39" s="14"/>
+      <c r="P39" s="21"/>
+      <c r="Q39" s="4"/>
+      <c r="R39" s="4"/>
+      <c r="S39" s="4"/>
+      <c r="T39" s="4"/>
+    </row>
+    <row r="40" spans="4:20" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D40" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="4"/>
+      <c r="H40" s="15"/>
+      <c r="I40" s="4"/>
+      <c r="J40" s="4"/>
+      <c r="K40" s="4"/>
+      <c r="L40" s="4"/>
+      <c r="M40" s="4"/>
+      <c r="N40" s="4"/>
+      <c r="O40" s="14"/>
+      <c r="P40" s="21"/>
+      <c r="Q40" s="4"/>
+      <c r="R40" s="4"/>
+      <c r="S40" s="4"/>
+      <c r="T40" s="4"/>
+    </row>
+    <row r="41" spans="4:20" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D41" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="4"/>
+      <c r="H41" s="15"/>
+      <c r="I41" s="4"/>
+      <c r="J41" s="4"/>
+      <c r="K41" s="4"/>
+      <c r="L41" s="4"/>
+      <c r="M41" s="4"/>
+      <c r="N41" s="4"/>
+      <c r="O41" s="14"/>
+      <c r="P41" s="21"/>
+      <c r="Q41" s="4"/>
+      <c r="R41" s="4"/>
+      <c r="S41" s="4"/>
+      <c r="T41" s="4"/>
+    </row>
+    <row r="42" spans="4:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D42" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="E42" s="4"/>
+      <c r="F42" s="15"/>
+      <c r="G42" s="4"/>
+      <c r="H42" s="4"/>
+      <c r="I42" s="4"/>
+      <c r="J42" s="15"/>
+      <c r="K42" s="4"/>
+      <c r="L42" s="4"/>
+      <c r="M42" s="4"/>
+      <c r="N42" s="4"/>
+      <c r="O42" s="4"/>
+      <c r="P42" s="4"/>
+      <c r="Q42" s="4"/>
+      <c r="R42" s="4"/>
+      <c r="S42" s="4"/>
+      <c r="T42" s="4"/>
+    </row>
+    <row r="43" spans="4:20" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D43" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="4"/>
+      <c r="H43" s="15"/>
+      <c r="I43" s="4"/>
+      <c r="J43" s="4"/>
+      <c r="K43" s="4"/>
+      <c r="L43" s="4"/>
+      <c r="M43" s="4"/>
+      <c r="N43" s="4"/>
+      <c r="O43" s="4"/>
+      <c r="P43" s="14"/>
+      <c r="Q43" s="4"/>
+      <c r="R43" s="4"/>
+      <c r="S43" s="4"/>
+      <c r="T43" s="4"/>
+    </row>
+    <row r="44" spans="4:20" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D44" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
+      <c r="G44" s="4"/>
+      <c r="H44" s="15"/>
+      <c r="I44" s="4"/>
+      <c r="J44" s="4"/>
+      <c r="K44" s="4"/>
+      <c r="L44" s="4"/>
+      <c r="M44" s="4"/>
+      <c r="N44" s="4"/>
+      <c r="O44" s="15"/>
+      <c r="P44" s="14"/>
+      <c r="Q44" s="4"/>
+      <c r="R44" s="4"/>
+      <c r="S44" s="4"/>
+      <c r="T44" s="4"/>
+    </row>
+    <row r="45" spans="4:20" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D45" s="16" t="s">
+        <v>132</v>
+      </c>
+      <c r="E45" s="4"/>
+      <c r="F45" s="15"/>
+      <c r="G45" s="4"/>
+      <c r="H45" s="4"/>
+      <c r="I45" s="4"/>
+      <c r="J45" s="15"/>
+      <c r="K45" s="4"/>
+      <c r="L45" s="4"/>
+      <c r="M45" s="4"/>
+      <c r="N45" s="4"/>
+      <c r="O45" s="4"/>
+      <c r="P45" s="4"/>
+      <c r="Q45" s="4"/>
+      <c r="R45" s="4"/>
+      <c r="S45" s="4"/>
+      <c r="T45" s="4"/>
+    </row>
+    <row r="46" spans="4:20" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D46" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
+      <c r="G46" s="4"/>
+      <c r="H46" s="15"/>
+      <c r="I46" s="4"/>
+      <c r="J46" s="4"/>
+      <c r="K46" s="4"/>
+      <c r="L46" s="4"/>
+      <c r="M46" s="4"/>
+      <c r="N46" s="4"/>
+      <c r="O46" s="15"/>
+      <c r="P46" s="4"/>
+      <c r="Q46" s="14"/>
+      <c r="R46" s="4"/>
+      <c r="S46" s="4"/>
+      <c r="T46" s="4"/>
+    </row>
+    <row r="47" spans="4:20" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D47" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="E47" s="4"/>
+      <c r="F47" s="4"/>
+      <c r="G47" s="4"/>
+      <c r="H47" s="15"/>
+      <c r="I47" s="4"/>
+      <c r="J47" s="4"/>
+      <c r="K47" s="4"/>
+      <c r="L47" s="4"/>
+      <c r="M47" s="4"/>
+      <c r="N47" s="4"/>
+      <c r="O47" s="15"/>
+      <c r="P47" s="4"/>
+      <c r="Q47" s="14"/>
+      <c r="R47" s="4"/>
+      <c r="S47" s="4"/>
+      <c r="T47" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="D4:D6"/>
+    <mergeCell ref="E4:T4"/>
+    <mergeCell ref="E5:H5"/>
+    <mergeCell ref="I5:L5"/>
+    <mergeCell ref="M5:P5"/>
+    <mergeCell ref="Q5:T5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>